<commit_message>
Refactor CartTableComponent path, update pom.xml with Allure, cleanup screenshots, update test data
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>Email</t>
   </si>
@@ -433,6 +433,12 @@
   </si>
   <si>
     <t>o524jxmo8uht</t>
+  </si>
+  <si>
+    <t>herbert.purdy@gmail.com</t>
+  </si>
+  <si>
+    <t>rr5cak4nbtd</t>
   </si>
 </sst>
 </file>
@@ -762,7 +768,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
@@ -1324,6 +1330,14 @@
         <v>135</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A24" r:id="rId1" xr:uid="{5C4675F8-06AD-48E0-BCE0-425D40ECFF3F}"/>

</xml_diff>